<commit_message>
Minor changes on merge with WB data
Adds information about income and regional groups for Micronesia (Federated States of), United Republic of Tanzania, and Viet Nam
</commit_message>
<xml_diff>
--- a/ndcs_clean.xlsx
+++ b/ndcs_clean.xlsx
@@ -16794,10 +16794,26 @@
       <c r="AX66" t="n">
         <v>0</v>
       </c>
-      <c r="AY66" t="inlineStr"/>
-      <c r="AZ66" t="inlineStr"/>
-      <c r="BA66" t="inlineStr"/>
-      <c r="BB66" t="inlineStr"/>
+      <c r="AY66" t="inlineStr">
+        <is>
+          <t>VNM</t>
+        </is>
+      </c>
+      <c r="AZ66" t="inlineStr">
+        <is>
+          <t>East Asia &amp; Pacific</t>
+        </is>
+      </c>
+      <c r="BA66" t="inlineStr">
+        <is>
+          <t>Lower middle income</t>
+        </is>
+      </c>
+      <c r="BB66" t="inlineStr">
+        <is>
+          <t>IBRD</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -20758,10 +20774,26 @@
       <c r="AX82" t="n">
         <v>0</v>
       </c>
-      <c r="AY82" t="inlineStr"/>
-      <c r="AZ82" t="inlineStr"/>
-      <c r="BA82" t="inlineStr"/>
-      <c r="BB82" t="inlineStr"/>
+      <c r="AY82" t="inlineStr">
+        <is>
+          <t>TZA</t>
+        </is>
+      </c>
+      <c r="AZ82" t="inlineStr">
+        <is>
+          <t>Sub-Saharan Africa</t>
+        </is>
+      </c>
+      <c r="BA82" t="inlineStr">
+        <is>
+          <t>Lower middle income</t>
+        </is>
+      </c>
+      <c r="BB82" t="inlineStr">
+        <is>
+          <t>IDA</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -45973,10 +46005,26 @@
       <c r="AX184" t="n">
         <v>0</v>
       </c>
-      <c r="AY184" t="inlineStr"/>
-      <c r="AZ184" t="inlineStr"/>
-      <c r="BA184" t="inlineStr"/>
-      <c r="BB184" t="inlineStr"/>
+      <c r="AY184" t="inlineStr">
+        <is>
+          <t>FSM</t>
+        </is>
+      </c>
+      <c r="AZ184" t="inlineStr">
+        <is>
+          <t>East Asia &amp; Pacific</t>
+        </is>
+      </c>
+      <c r="BA184" t="inlineStr">
+        <is>
+          <t>Lower middle income</t>
+        </is>
+      </c>
+      <c r="BB184" t="inlineStr">
+        <is>
+          <t>IDA</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">

</xml_diff>